<commit_message>
added respective Cit_Par file for every motion
</commit_message>
<xml_diff>
--- a/Flight_datasheet_cmdelta_cmalpha_clcd.xlsx
+++ b/Flight_datasheet_cmdelta_cmalpha_clcd.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emili\Documents\TU DELFT\Year 3\Q3\SVV\FLight dynamics report\SVV_FD_B23\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A52CA20-2E95-41D3-9CAD-3E828B9034E8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A83B4895-CC2F-4B64-A0D3-EDB73C78917B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5064" yWindow="348" windowWidth="11460" windowHeight="10968" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5064" yWindow="348" windowWidth="11460" windowHeight="10968" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1234,6 +1234,14 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$F$28:$F$33</c:f>
@@ -3751,8 +3759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W88"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S68" sqref="S68"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A42" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q68" sqref="Q68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4638,7 +4646,7 @@
         <v>62738.926836485196</v>
       </c>
       <c r="O29">
-        <f t="shared" ref="O28:O33" si="11">R29+S29</f>
+        <f t="shared" ref="O29:O33" si="11">R29+S29</f>
         <v>7047.01</v>
       </c>
       <c r="P29">
@@ -4646,7 +4654,7 @@
         <v>7041.332894315452</v>
       </c>
       <c r="Q29">
-        <f t="shared" ref="Q28:Q33" si="12">N29-O29*SIN(RADIANS(F29))</f>
+        <f t="shared" ref="Q29:Q33" si="12">N29-O29*SIN(RADIANS(F29))</f>
         <v>62456.117693190325</v>
       </c>
       <c r="R29">
@@ -4656,15 +4664,15 @@
         <v>3978.92</v>
       </c>
       <c r="T29">
-        <f t="shared" ref="T28:T33" si="13">1.225*(((288.15-0.0065*(D29*0.3048))/288.15)^(-9.80665/(-0.0065*287.05)-1))</f>
+        <f t="shared" ref="T29:T33" si="13">1.225*(((288.15-0.0065*(D29*0.3048))/288.15)^(-9.80665/(-0.0065*287.05)-1))</f>
         <v>0.84859186310327495</v>
       </c>
       <c r="U29">
-        <f t="shared" ref="U28:U33" si="14">E29*0.5144444444</f>
+        <f t="shared" ref="U29:U33" si="14">E29*0.5144444444</f>
         <v>111.6344444348</v>
       </c>
       <c r="V29">
-        <f t="shared" ref="V28:V33" si="15">Q29/(0.5*T29*U29^2*$B$20)</f>
+        <f t="shared" ref="V29:V33" si="15">Q29/(0.5*T29*U29^2*$B$20)</f>
         <v>0.32810072174714611</v>
       </c>
       <c r="W29">
@@ -6437,8 +6445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86FC5488-0BFE-4566-95C3-43278896809C}">
   <dimension ref="A1:W12"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6447,6 +6455,7 @@
     <col min="9" max="9" width="12.88671875" customWidth="1"/>
     <col min="11" max="11" width="13.44140625" customWidth="1"/>
     <col min="13" max="13" width="14.33203125" customWidth="1"/>
+    <col min="23" max="23" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.3">
@@ -6613,21 +6622,21 @@
       </c>
       <c r="N4">
         <f>Q4+R4</f>
-        <v>7499.77</v>
+        <v>3821.05</v>
       </c>
       <c r="O4">
         <f>N4*COS(RADIANS(E4))</f>
-        <v>7442.3534963274205</v>
+        <v>3791.7969253912975</v>
       </c>
       <c r="P4">
         <f>M4-N4*SIN(RADIANS(E4))</f>
-        <v>60421.362631050244</v>
+        <v>60875.694625075645</v>
       </c>
       <c r="Q4">
-        <v>3697.8</v>
+        <v>1774.73</v>
       </c>
       <c r="R4">
-        <v>3801.97</v>
+        <v>2046.32</v>
       </c>
       <c r="S4">
         <f>1.225*(((288.15-0.0065*(C4*0.3048))/288.15)^(-9.80665/(-0.0065*287.05)-1))</f>
@@ -6639,15 +6648,15 @@
       </c>
       <c r="U4">
         <f>P4/(0.5*S4*T4^2*$D$11)</f>
-        <v>0.42716106577927948</v>
+        <v>0.43037305786841162</v>
       </c>
       <c r="V4">
         <f>O4/(0.5*S4*T4^2*$D$11)</f>
-        <v>5.2615226022123048E-2</v>
+        <v>2.6806876663128774E-2</v>
       </c>
       <c r="W4">
         <f>V4-(U4^2)/(PI()*7.11111*0.8)</f>
-        <v>4.2405688573615034E-2</v>
+        <v>1.6443222897783629E-2</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.3">
@@ -6676,15 +6685,21 @@
       </c>
       <c r="N5">
         <f>Q5+R5</f>
-        <v>0</v>
+        <v>4067.21</v>
       </c>
       <c r="O5">
         <f t="shared" ref="O5:O9" si="2">N5*COS(RADIANS(E5))</f>
-        <v>0</v>
+        <v>4017.5931239692559</v>
       </c>
       <c r="P5">
         <f t="shared" ref="P5:P9" si="3">M5-N5*SIN(RADIANS(E5))</f>
-        <v>61293.588524831408</v>
+        <v>60660.230273653644</v>
+      </c>
+      <c r="Q5">
+        <v>1892.53</v>
+      </c>
+      <c r="R5">
+        <v>2174.6799999999998</v>
       </c>
       <c r="S5">
         <f t="shared" ref="S5:S9" si="4">1.225*(((288.15-0.0065*(C5*0.3048))/288.15)^(-9.80665/(-0.0065*287.05)-1))</f>
@@ -6696,15 +6711,15 @@
       </c>
       <c r="U5">
         <f t="shared" ref="U5:U9" si="6">P5/(0.5*S5*T5^2*$D$11)</f>
-        <v>0.62945427422597178</v>
+        <v>0.62295000407447587</v>
       </c>
       <c r="V5">
         <f t="shared" ref="V5:V9" si="7">O5/(0.5*S5*T5^2*$D$11)</f>
-        <v>0</v>
+        <v>4.1258657305711703E-2</v>
       </c>
       <c r="W5">
         <f t="shared" ref="W5:W9" si="8">V5-(U5^2)/(PI()*7.11111*0.8)</f>
-        <v>-2.2169255949309914E-2</v>
+        <v>1.9545192473857231E-2</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.3">
@@ -6732,16 +6747,22 @@
         <v>61205.361207309244</v>
       </c>
       <c r="N6">
-        <f t="shared" ref="N5:N9" si="9">Q6+R6</f>
-        <v>0</v>
+        <f t="shared" ref="N6:N9" si="9">Q6+R6</f>
+        <v>3752.79</v>
       </c>
       <c r="O6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>3737.00022374335</v>
       </c>
       <c r="P6">
         <f t="shared" si="3"/>
-        <v>61205.361207309244</v>
+        <v>60861.468619657011</v>
+      </c>
+      <c r="Q6">
+        <v>1740.55</v>
+      </c>
+      <c r="R6">
+        <v>2012.24</v>
       </c>
       <c r="S6">
         <f t="shared" si="4"/>
@@ -6753,15 +6774,15 @@
       </c>
       <c r="U6">
         <f t="shared" si="6"/>
-        <v>0.38805424221215346</v>
+        <v>0.38587389436563463</v>
       </c>
       <c r="V6">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>2.3693329495426511E-2</v>
       </c>
       <c r="W6">
         <f t="shared" si="8"/>
-        <v>-8.4257314835718376E-3</v>
+        <v>1.5362014787443057E-2</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.3">
@@ -6790,15 +6811,21 @@
       </c>
       <c r="N7">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>3746.41</v>
       </c>
       <c r="O7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>3734.164239221026</v>
       </c>
       <c r="P7">
         <f t="shared" si="3"/>
-        <v>61022.499573553323</v>
+        <v>60719.835861452164</v>
+      </c>
+      <c r="Q7">
+        <v>1740.41</v>
+      </c>
+      <c r="R7">
+        <v>2006</v>
       </c>
       <c r="S7">
         <f t="shared" si="4"/>
@@ -6810,15 +6837,15 @@
       </c>
       <c r="U7">
         <f t="shared" si="6"/>
-        <v>0.37223421764716219</v>
+        <v>0.37038798403052109</v>
       </c>
       <c r="V7">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>2.2778216458947832E-2</v>
       </c>
       <c r="W7">
         <f t="shared" si="8"/>
-        <v>-7.7527419722753805E-3</v>
+        <v>1.510218896338434E-2</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.3">
@@ -6847,15 +6874,21 @@
       </c>
       <c r="N8">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>3775.1899999999996</v>
       </c>
       <c r="O8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>3759.8990131922415</v>
       </c>
       <c r="P8">
         <f t="shared" si="3"/>
-        <v>60965.184993470168</v>
+        <v>60625.745828528925</v>
+      </c>
+      <c r="Q8">
+        <v>1757.11</v>
+      </c>
+      <c r="R8">
+        <v>2018.08</v>
       </c>
       <c r="S8">
         <f t="shared" si="4"/>
@@ -6867,15 +6900,15 @@
       </c>
       <c r="U8">
         <f t="shared" si="6"/>
-        <v>0.37991336132465564</v>
+        <v>0.37779809711063128</v>
       </c>
       <c r="V8">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>2.343035410285586E-2</v>
       </c>
       <c r="W8">
         <f t="shared" si="8"/>
-        <v>-8.0759175984166497E-3</v>
+        <v>1.5444115600199378E-2</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.3">
@@ -6904,15 +6937,21 @@
       </c>
       <c r="N9">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>3701.85</v>
       </c>
       <c r="O9">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>3686.1897809458433</v>
       </c>
       <c r="P9">
         <f t="shared" si="3"/>
-        <v>60599.878531211412</v>
+        <v>60259.733971721718</v>
+      </c>
+      <c r="Q9">
+        <v>1732.3</v>
+      </c>
+      <c r="R9">
+        <v>1969.55</v>
       </c>
       <c r="S9">
         <f t="shared" si="4"/>
@@ -6924,15 +6963,15 @@
       </c>
       <c r="U9">
         <f t="shared" si="6"/>
-        <v>0.38547535671077471</v>
+        <v>0.38331169980946611</v>
       </c>
       <c r="V9">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>2.3447824569184109E-2</v>
       </c>
       <c r="W9">
         <f t="shared" si="8"/>
-        <v>-8.3141141250022664E-3</v>
+        <v>1.5226782048637939E-2</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.3">

</xml_diff>